<commit_message>
post rhizodep update bug correction
</commit_message>
<xml_diff>
--- a/simulations/single_plant/inputs/Scenarios_24-09-13.xlsx
+++ b/simulations/single_plant/inputs/Scenarios_24-09-13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\simulations\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\simulations\single_plant\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040B088-EA4F-468F-B08C-A5BADD44213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32AF937-A2B1-4BFA-940C-83E2F970CA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2415,48 +2415,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2737,13 +2737,13 @@
   <dimension ref="A1:Z222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="J42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
@@ -20575,7 +20575,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>

</xml_diff>